<commit_message>
Improve accuracy of driver data by incorporating employee details
Updates "Driver", "EmployeeID", "Status", "JobSite", "FirstSeen", "LastSeen", "Hours", and "Location" fields in filtered_driving_data JSON files.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: b83b866c-5b8f-4d82-9fde-612e7a355315
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f2699832-8135-4557-9ec0-8d4d723b9ba2/46f6bd85-7f9f-4e1c-a550-937835b487be.jpg
</commit_message>
<xml_diff>
--- a/reports/daily_driver_reports/DAILY_DRIVER_REPORT_2025_05_18.xlsx
+++ b/reports/daily_driver_reports/DAILY_DRIVER_REPORT_2025_05_18.xlsx
@@ -37,7 +37,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -48,6 +48,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00DDDDDD"/>
         <bgColor rgb="00DDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFDD"/>
+        <bgColor rgb="00FFFFDD"/>
       </patternFill>
     </fill>
   </fills>
@@ -69,7 +75,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -78,6 +84,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -454,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,112 +558,1148 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>TROY MALETTE</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr"/>
+      <c r="C5" s="4" t="inlineStr"/>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E5" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5" t="inlineStr"/>
+      <c r="I5" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J5" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K5" s="5" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>LORENZO APARICIO</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr"/>
+      <c r="C6" s="4" t="inlineStr"/>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5" t="inlineStr"/>
+      <c r="I6" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J6" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K6" s="5" t="n"/>
+    </row>
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
         <is>
+          <t>Aaron Moore</t>
+        </is>
+      </c>
+      <c r="B7" s="5" t="inlineStr"/>
+      <c r="C7" s="4" t="inlineStr"/>
+      <c r="D7" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5" t="inlineStr"/>
+      <c r="I7" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J7" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K7" s="5" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="inlineStr">
+        <is>
+          <t>ALEJANDRO LOZANO ACOSTA</t>
+        </is>
+      </c>
+      <c r="B8" s="5" t="inlineStr"/>
+      <c r="C8" s="4" t="inlineStr"/>
+      <c r="D8" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E8" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F8" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5" t="inlineStr"/>
+      <c r="I8" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J8" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K8" s="5" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="inlineStr">
+        <is>
+          <t>JOSE J RIVERA</t>
+        </is>
+      </c>
+      <c r="B9" s="5" t="inlineStr"/>
+      <c r="C9" s="4" t="inlineStr"/>
+      <c r="D9" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E9" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F9" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5" t="inlineStr"/>
+      <c r="I9" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J9" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K9" s="5" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="inlineStr">
+        <is>
+          <t>Adam Goode</t>
+        </is>
+      </c>
+      <c r="B10" s="5" t="inlineStr"/>
+      <c r="C10" s="4" t="inlineStr"/>
+      <c r="D10" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E10" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F10" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5" t="inlineStr"/>
+      <c r="I10" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J10" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K10" s="5" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="inlineStr">
+        <is>
+          <t>JUAN LOPEZ-VAZQUEZ</t>
+        </is>
+      </c>
+      <c r="B11" s="5" t="inlineStr"/>
+      <c r="C11" s="4" t="inlineStr"/>
+      <c r="D11" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E11" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F11" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5" t="inlineStr"/>
+      <c r="I11" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J11" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K11" s="5" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>LEROY ARNOLD</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="inlineStr"/>
+      <c r="C12" s="4" t="inlineStr"/>
+      <c r="D12" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E12" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F12" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5" t="inlineStr"/>
+      <c r="I12" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J12" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K12" s="5" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="inlineStr">
+        <is>
+          <t>VICK ADHIKARI</t>
+        </is>
+      </c>
+      <c r="B13" s="5" t="inlineStr"/>
+      <c r="C13" s="4" t="inlineStr"/>
+      <c r="D13" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E13" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F13" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5" t="inlineStr"/>
+      <c r="I13" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J13" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K13" s="5" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="inlineStr">
+        <is>
+          <t>Matt Shaylor</t>
+        </is>
+      </c>
+      <c r="B14" s="5" t="inlineStr"/>
+      <c r="C14" s="4" t="inlineStr"/>
+      <c r="D14" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E14" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F14" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="5" t="inlineStr"/>
+      <c r="I14" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J14" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K14" s="5" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="inlineStr">
+        <is>
+          <t>Hector Bonilla</t>
+        </is>
+      </c>
+      <c r="B15" s="5" t="inlineStr"/>
+      <c r="C15" s="4" t="inlineStr"/>
+      <c r="D15" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E15" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F15" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5" t="inlineStr"/>
+      <c r="I15" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J15" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K15" s="5" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
+          <t>RAFAEL MURATALLA</t>
+        </is>
+      </c>
+      <c r="B16" s="5" t="inlineStr"/>
+      <c r="C16" s="4" t="inlineStr"/>
+      <c r="D16" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E16" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F16" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="5" t="inlineStr"/>
+      <c r="I16" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J16" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K16" s="5" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="inlineStr">
+        <is>
+          <t>SEYMORE HUNT</t>
+        </is>
+      </c>
+      <c r="B17" s="5" t="inlineStr"/>
+      <c r="C17" s="4" t="inlineStr"/>
+      <c r="D17" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E17" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F17" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="5" t="inlineStr"/>
+      <c r="I17" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J17" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K17" s="5" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="inlineStr">
+        <is>
+          <t>JUAN P RODRIGUEZ</t>
+        </is>
+      </c>
+      <c r="B18" s="5" t="inlineStr"/>
+      <c r="C18" s="4" t="inlineStr"/>
+      <c r="D18" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E18" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F18" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G18" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="5" t="inlineStr"/>
+      <c r="I18" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J18" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K18" s="5" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="inlineStr">
+        <is>
+          <t>URIEL GARCIA-ANDRADE</t>
+        </is>
+      </c>
+      <c r="B19" s="5" t="inlineStr"/>
+      <c r="C19" s="4" t="inlineStr"/>
+      <c r="D19" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E19" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F19" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="5" t="inlineStr"/>
+      <c r="I19" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J19" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K19" s="5" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="inlineStr">
+        <is>
+          <t>JUAN RUIZ</t>
+        </is>
+      </c>
+      <c r="B20" s="5" t="inlineStr"/>
+      <c r="C20" s="4" t="inlineStr"/>
+      <c r="D20" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E20" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F20" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="5" t="inlineStr"/>
+      <c r="I20" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J20" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K20" s="5" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="inlineStr">
+        <is>
+          <t>ROBERT BERRYHILL</t>
+        </is>
+      </c>
+      <c r="B21" s="5" t="inlineStr"/>
+      <c r="C21" s="4" t="inlineStr"/>
+      <c r="D21" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E21" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F21" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G21" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="5" t="inlineStr"/>
+      <c r="I21" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J21" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K21" s="5" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="inlineStr">
+        <is>
+          <t>SABINO IBARRA</t>
+        </is>
+      </c>
+      <c r="B22" s="5" t="inlineStr"/>
+      <c r="C22" s="4" t="inlineStr"/>
+      <c r="D22" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E22" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F22" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="5" t="inlineStr"/>
+      <c r="I22" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J22" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K22" s="5" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="inlineStr">
+        <is>
+          <t>LUIS MURCIA ORELLANA</t>
+        </is>
+      </c>
+      <c r="B23" s="5" t="inlineStr"/>
+      <c r="C23" s="4" t="inlineStr"/>
+      <c r="D23" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E23" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F23" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="5" t="inlineStr"/>
+      <c r="I23" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J23" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K23" s="5" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="inlineStr">
+        <is>
+          <t>Roger Doddy</t>
+        </is>
+      </c>
+      <c r="B24" s="5" t="inlineStr"/>
+      <c r="C24" s="4" t="inlineStr"/>
+      <c r="D24" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E24" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F24" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="5" t="inlineStr"/>
+      <c r="I24" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J24" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K24" s="5" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="4" t="inlineStr">
+        <is>
+          <t>ISAAC ROMERO</t>
+        </is>
+      </c>
+      <c r="B25" s="5" t="inlineStr"/>
+      <c r="C25" s="4" t="inlineStr"/>
+      <c r="D25" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E25" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F25" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="5" t="inlineStr"/>
+      <c r="I25" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J25" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K25" s="5" t="n"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="inlineStr">
+        <is>
+          <t>JOSE BAUTISTA</t>
+        </is>
+      </c>
+      <c r="B26" s="5" t="inlineStr"/>
+      <c r="C26" s="4" t="inlineStr"/>
+      <c r="D26" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E26" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F26" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G26" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="5" t="inlineStr"/>
+      <c r="I26" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J26" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K26" s="5" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="inlineStr">
+        <is>
+          <t>Nagesh Kumar</t>
+        </is>
+      </c>
+      <c r="B27" s="5" t="inlineStr"/>
+      <c r="C27" s="4" t="inlineStr"/>
+      <c r="D27" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E27" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F27" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G27" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="5" t="inlineStr"/>
+      <c r="I27" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J27" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K27" s="5" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="inlineStr">
+        <is>
+          <t>Sam Abunemeh</t>
+        </is>
+      </c>
+      <c r="B28" s="5" t="inlineStr"/>
+      <c r="C28" s="4" t="inlineStr"/>
+      <c r="D28" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E28" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F28" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="5" t="inlineStr"/>
+      <c r="I28" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J28" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K28" s="5" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="4" t="inlineStr">
+        <is>
+          <t>JOVAN ESPINOZA-CASILLAS</t>
+        </is>
+      </c>
+      <c r="B29" s="5" t="inlineStr"/>
+      <c r="C29" s="4" t="inlineStr"/>
+      <c r="D29" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E29" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F29" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="5" t="inlineStr"/>
+      <c r="I29" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J29" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K29" s="5" t="n"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="inlineStr">
+        <is>
+          <t>ROBERTO GUERRERO JR</t>
+        </is>
+      </c>
+      <c r="B30" s="5" t="inlineStr"/>
+      <c r="C30" s="4" t="inlineStr"/>
+      <c r="D30" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E30" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F30" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G30" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="5" t="inlineStr"/>
+      <c r="I30" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J30" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K30" s="5" t="n"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="4" t="inlineStr">
+        <is>
+          <t>CHASE JONES</t>
+        </is>
+      </c>
+      <c r="B31" s="5" t="inlineStr"/>
+      <c r="C31" s="4" t="inlineStr"/>
+      <c r="D31" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E31" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F31" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="5" t="inlineStr"/>
+      <c r="I31" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J31" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K31" s="5" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="inlineStr">
+        <is>
+          <t>Ammar Elhamad</t>
+        </is>
+      </c>
+      <c r="B32" s="5" t="inlineStr"/>
+      <c r="C32" s="4" t="inlineStr"/>
+      <c r="D32" s="5" t="inlineStr">
+        <is>
+          <t>EARLY END</t>
+        </is>
+      </c>
+      <c r="E32" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="F32" s="5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="G32" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="5" t="inlineStr"/>
+      <c r="I32" s="5" t="n">
+        <v>540</v>
+      </c>
+      <c r="J32" s="5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="K32" s="5" t="n"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="inlineStr">
+        <is>
           <t>SUMMARY</t>
         </is>
       </c>
-      <c r="B7" s="5" t="n"/>
-      <c r="C7" s="5" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="inlineStr">
+      <c r="B35" s="7" t="n"/>
+      <c r="C35" s="7" t="n"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="8" t="inlineStr">
         <is>
           <t>Total Drivers:</t>
         </is>
       </c>
-      <c r="B8" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="5" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="inlineStr">
+      <c r="B36" s="7" t="n">
+        <v>28</v>
+      </c>
+      <c r="C36" s="7" t="n"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="8" t="inlineStr">
         <is>
           <t>On Time:</t>
         </is>
       </c>
-      <c r="B9" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="5" t="inlineStr">
+      <c r="B37" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" s="7" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="6" t="inlineStr">
+    <row r="38">
+      <c r="A38" s="8" t="inlineStr">
         <is>
           <t>Late:</t>
         </is>
       </c>
-      <c r="B10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="5" t="inlineStr">
+      <c r="B38" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" s="7" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="6" t="inlineStr">
+    <row r="39">
+      <c r="A39" s="8" t="inlineStr">
         <is>
           <t>Early End:</t>
         </is>
       </c>
-      <c r="B11" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="5" t="inlineStr">
+      <c r="B39" s="7" t="n">
+        <v>28</v>
+      </c>
+      <c r="C39" s="7" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="8" t="inlineStr">
+        <is>
+          <t>Not On Job:</t>
+        </is>
+      </c>
+      <c r="B40" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" s="7" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>Not On Job:</t>
-        </is>
-      </c>
-      <c r="B12" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="5" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="n"/>
-      <c r="B13" s="5" t="n"/>
-      <c r="C13" s="5" t="n"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="6" t="inlineStr">
+    <row r="41">
+      <c r="A41" s="8" t="n"/>
+      <c r="B41" s="7" t="n"/>
+      <c r="C41" s="7" t="n"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="8" t="inlineStr">
         <is>
           <t>Average Late Minutes:</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="5" t="n"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="6" t="inlineStr">
+      <c r="B42" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" s="7" t="n"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="8" t="inlineStr">
         <is>
           <t>Average Early End Minutes:</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="5" t="n"/>
+      <c r="B43" s="7" t="n">
+        <v>540</v>
+      </c>
+      <c r="C43" s="7" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>